<commit_message>
Add linked data fragment support with graphdb backend.
</commit_message>
<xml_diff>
--- a/molgenis-fair/src/test/resources/FDP.xlsx
+++ b/molgenis-fair/src/test/resources/FDP.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="28125"/>
   <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="13800" tabRatio="500" firstSheet="3" activeTab="7"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="13800" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="attributes" sheetId="1" r:id="rId1"/>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="536" uniqueCount="158">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="542" uniqueCount="163">
   <si>
     <t>entity</t>
   </si>
@@ -504,6 +504,21 @@
   </si>
   <si>
     <t>text/turtle</t>
+  </si>
+  <si>
+    <t>http://www.re3data.org/schema/3-0#dataCatalog</t>
+  </si>
+  <si>
+    <t>r3d:dataCatalog</t>
+  </si>
+  <si>
+    <t>R3D</t>
+  </si>
+  <si>
+    <t>dataCatalog</t>
+  </si>
+  <si>
+    <t>ldp:contains,r3d:dataCatalog</t>
   </si>
 </sst>
 </file>
@@ -847,8 +862,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H1007"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="H2" sqref="H2"/>
+    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
+      <selection activeCell="B18" sqref="B18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="13.5" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0"/>
@@ -1189,7 +1204,7 @@
         <v>8</v>
       </c>
       <c r="B18" s="6" t="s">
-        <v>73</v>
+        <v>162</v>
       </c>
       <c r="C18" s="4" t="s">
         <v>75</v>
@@ -7905,10 +7920,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F29"/>
+  <dimension ref="A1:F30"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+    <sheetView topLeftCell="A3" workbookViewId="0">
+      <selection activeCell="B30" sqref="B30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="13.5" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0"/>
@@ -8496,6 +8511,26 @@
         <v>84</v>
       </c>
       <c r="F29" s="6" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6" ht="15" customHeight="1">
+      <c r="A30" t="s">
+        <v>159</v>
+      </c>
+      <c r="B30" t="s">
+        <v>158</v>
+      </c>
+      <c r="C30" s="6" t="s">
+        <v>161</v>
+      </c>
+      <c r="D30" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="E30" s="6" t="s">
+        <v>160</v>
+      </c>
+      <c r="F30" s="6" t="s">
         <v>35</v>
       </c>
     </row>
@@ -8837,7 +8872,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M2"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="K3" sqref="K3"/>
     </sheetView>
   </sheetViews>

</xml_diff>